<commit_message>
this commit is From other user
</commit_message>
<xml_diff>
--- a/File1.xlsx
+++ b/File1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitagrawal8/Gitstuff/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitagrawal8/GITDemo/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4813FB51-EB8E-914C-AC02-4AE4872B93EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6101ACC-7E57-4F48-8734-3B0827170718}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16300" xr2:uid="{0757B9AD-F0F5-9948-A328-08DD6F26C94B}"/>
   </bookViews>
@@ -35,9 +35,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Test1</t>
+  </si>
+  <si>
+    <t>updated file</t>
   </si>
 </sst>
 </file>
@@ -389,10 +392,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7300FF86-74E3-324B-8E00-98AD3E35866A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -402,6 +405,11 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>